<commit_message>
Output file min error highlighted
</commit_message>
<xml_diff>
--- a/output_final_updated.xlsx
+++ b/output_final_updated.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hamza\Machine Learning Assignments\NSGA-2-for-Feature-Selection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7A2FF45-4EDD-4D19-9A33-8B8FFE63740F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{974CC2F5-671D-4CA1-9964-9BBDAAD62334}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4641,12 +4641,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -4689,7 +4701,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -4718,6 +4730,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4764,7 +4778,7 @@
                   <a14:compatExt spid="_x0000_s7169"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-0000011C0000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0A00-0000011C0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5082,7 +5096,7 @@
   <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -5165,7 +5179,7 @@
       <c r="G2">
         <v>5.9738919247115971</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="10">
         <v>0.157894736842105</v>
       </c>
       <c r="I2">
@@ -5177,7 +5191,7 @@
       <c r="K2">
         <v>11</v>
       </c>
-      <c r="L2">
+      <c r="L2" s="11">
         <v>0.105263157894736</v>
       </c>
       <c r="M2">
@@ -5200,7 +5214,7 @@
       <c r="E3">
         <v>9.6774193548387094E-2</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="10">
         <v>4.9539170506912422E-2</v>
       </c>
       <c r="G3">
@@ -5247,7 +5261,7 @@
       <c r="G4">
         <v>3.9696969696969702</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="10">
         <v>4.54545454545454E-2</v>
       </c>
       <c r="I4">
@@ -5288,7 +5302,7 @@
       <c r="G5">
         <v>11</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="10">
         <v>0.24137931034482701</v>
       </c>
       <c r="I5">
@@ -5341,7 +5355,7 @@
       <c r="K6">
         <v>33</v>
       </c>
-      <c r="L6">
+      <c r="L6" s="10">
         <v>4.54545454545454E-2</v>
       </c>
       <c r="M6">
@@ -5370,7 +5384,7 @@
       <c r="G7">
         <v>104.30769230769231</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="10">
         <v>0.19230769230769201</v>
       </c>
       <c r="I7">
@@ -5411,7 +5425,7 @@
       <c r="G8">
         <v>6.9356223175965663</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="10">
         <v>4.91803278688525E-2</v>
       </c>
       <c r="I8">
@@ -5452,7 +5466,7 @@
       <c r="G9">
         <v>19.6875</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="11">
         <v>0.133333333333333</v>
       </c>
       <c r="I9">
@@ -5464,7 +5478,7 @@
       <c r="K9">
         <v>46</v>
       </c>
-      <c r="L9">
+      <c r="L9" s="10">
         <v>6.6666666666666596E-2</v>
       </c>
       <c r="M9">
@@ -5487,7 +5501,7 @@
       <c r="E10">
         <v>0.47058823529411697</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="10">
         <v>0.38914027149321301</v>
       </c>
       <c r="G10">
@@ -5519,7 +5533,7 @@
       <c r="D11">
         <v>0.24166666666666661</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="10">
         <v>0.25862068965517199</v>
       </c>
       <c r="F11">
@@ -5563,7 +5577,7 @@
       <c r="G12">
         <v>5.7629290617848969</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="10">
         <v>0.1111111111111112</v>
       </c>
       <c r="I12">
@@ -5589,7 +5603,7 @@
       <c r="D13">
         <v>0.1727272727272727</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="10">
         <v>0.20689655172413701</v>
       </c>
       <c r="F13">
@@ -5633,13 +5647,13 @@
       <c r="G14">
         <v>1314.9230769230769</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="10">
         <v>0.33333333333333343</v>
       </c>
       <c r="I14">
         <v>1313</v>
       </c>
-      <c r="L14">
+      <c r="L14" s="11">
         <v>0.26666666666666672</v>
       </c>
       <c r="M14">
@@ -5674,7 +5688,7 @@
       <c r="I15">
         <v>70</v>
       </c>
-      <c r="L15">
+      <c r="L15" s="10">
         <v>0.26315789473684209</v>
       </c>
       <c r="M15">

</xml_diff>

<commit_message>
10 Runs and Research paper update
</commit_message>
<xml_diff>
--- a/output_final_updated.xlsx
+++ b/output_final_updated.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hamza\Machine Learning Assignments\NSGA-2-for-Feature-Selection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D436835-56ED-48C7-A4B7-6994EBBF1FDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79B9B4B5-0489-4D62-A01B-DBC2BCFB7BE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="832" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2729" uniqueCount="1494">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2935" uniqueCount="1497">
   <si>
     <t>Dataset</t>
   </si>
@@ -4588,9 +4588,6 @@
     <t>Glioma</t>
   </si>
   <si>
-    <t>Avg. of test error for all run</t>
-  </si>
-  <si>
     <t>CLL_SUB_111</t>
   </si>
   <si>
@@ -4604,6 +4601,18 @@
   </si>
   <si>
     <t xml:space="preserve">Breast </t>
+  </si>
+  <si>
+    <t>Avg. of test error from 10 runs</t>
+  </si>
+  <si>
+    <t>#Avg features for test</t>
+  </si>
+  <si>
+    <t>CLL_SUB_111,111</t>
+  </si>
+  <si>
+    <t>SRBCT_Split,83</t>
   </si>
 </sst>
 </file>
@@ -4793,13 +4802,13 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5161,10 +5170,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N40"/>
+  <dimension ref="A1:N170"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D10" zoomScale="90" zoomScaleNormal="72" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="90" zoomScaleNormal="72" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -5174,12 +5183,12 @@
     <col min="3" max="3" width="30.109375" customWidth="1"/>
     <col min="4" max="4" width="27.21875" customWidth="1"/>
     <col min="5" max="5" width="31.6640625" customWidth="1"/>
-    <col min="6" max="6" width="36.21875" customWidth="1"/>
-    <col min="7" max="7" width="19" customWidth="1"/>
+    <col min="6" max="6" width="26" customWidth="1"/>
+    <col min="7" max="7" width="33.44140625" customWidth="1"/>
     <col min="8" max="8" width="28.88671875" customWidth="1"/>
     <col min="9" max="9" width="32.44140625" customWidth="1"/>
-    <col min="10" max="10" width="48.5546875" customWidth="1"/>
-    <col min="11" max="11" width="22.77734375" customWidth="1"/>
+    <col min="10" max="10" width="58.88671875" customWidth="1"/>
+    <col min="11" max="11" width="58.21875" customWidth="1"/>
     <col min="12" max="12" width="40.88671875" customWidth="1"/>
     <col min="13" max="13" width="23.5546875" customWidth="1"/>
     <col min="14" max="14" width="26.6640625" customWidth="1"/>
@@ -5281,7 +5290,7 @@
       <c r="G3">
         <v>14.857142857142859</v>
       </c>
-      <c r="H3" s="16">
+      <c r="H3">
         <v>6.4516129032258104E-2</v>
       </c>
       <c r="I3">
@@ -5316,7 +5325,7 @@
       <c r="G4">
         <v>3.9696969696969702</v>
       </c>
-      <c r="H4" s="16">
+      <c r="H4">
         <v>9.0909090909090898E-2</v>
       </c>
       <c r="I4">
@@ -5386,13 +5395,13 @@
       <c r="G6">
         <v>20.5</v>
       </c>
-      <c r="H6" s="16">
+      <c r="H6">
         <v>0.31818181818181801</v>
       </c>
       <c r="I6">
         <v>20</v>
       </c>
-      <c r="J6" s="9">
+      <c r="J6" s="18">
         <v>4.54545454545454E-2</v>
       </c>
       <c r="K6">
@@ -5427,7 +5436,7 @@
       <c r="I7">
         <v>104</v>
       </c>
-      <c r="J7">
+      <c r="J7" s="18">
         <v>0.19230769230769201</v>
       </c>
       <c r="K7">
@@ -5456,13 +5465,13 @@
       <c r="G8">
         <v>6.9356223175965663</v>
       </c>
-      <c r="H8" s="16">
+      <c r="H8">
         <v>6.5573770491803199E-2</v>
       </c>
       <c r="I8">
         <v>7</v>
       </c>
-      <c r="J8" s="9">
+      <c r="J8" s="18">
         <v>4.91803278688525E-2</v>
       </c>
       <c r="K8">
@@ -5491,13 +5500,13 @@
       <c r="G9">
         <v>19.6875</v>
       </c>
-      <c r="H9" s="16">
+      <c r="H9">
         <v>0.266666666666666</v>
       </c>
       <c r="I9">
         <v>20</v>
       </c>
-      <c r="J9" s="9">
+      <c r="J9" s="18">
         <v>6.6666666666666596E-2</v>
       </c>
       <c r="K9">
@@ -5526,13 +5535,13 @@
       <c r="G10">
         <v>59.384615384615401</v>
       </c>
-      <c r="H10" s="16">
+      <c r="H10">
         <v>0.58823529411764697</v>
       </c>
       <c r="I10">
         <v>59</v>
       </c>
-      <c r="J10">
+      <c r="J10" s="18">
         <v>0.38235294117647001</v>
       </c>
       <c r="K10">
@@ -5561,13 +5570,13 @@
       <c r="G11">
         <v>116.3</v>
       </c>
-      <c r="H11" s="16">
+      <c r="H11">
         <v>0.34482758620689602</v>
       </c>
       <c r="I11">
         <v>116</v>
       </c>
-      <c r="J11">
+      <c r="J11" s="18">
         <v>0.31034482758620602</v>
       </c>
       <c r="K11">
@@ -5602,7 +5611,7 @@
       <c r="I12">
         <v>6</v>
       </c>
-      <c r="J12">
+      <c r="J12" s="18">
         <v>3.7037037037037E-2</v>
       </c>
       <c r="K12">
@@ -5631,13 +5640,13 @@
       <c r="G13">
         <v>183.4</v>
       </c>
-      <c r="H13" s="16">
+      <c r="H13">
         <v>0.2413793103448276</v>
       </c>
       <c r="I13">
         <v>184</v>
       </c>
-      <c r="J13">
+      <c r="J13" s="18">
         <v>0.29310344827586199</v>
       </c>
       <c r="K13">
@@ -5672,8 +5681,8 @@
       <c r="I14">
         <v>1313</v>
       </c>
-      <c r="J14" s="10">
-        <v>0.26666666666666672</v>
+      <c r="J14" s="18">
+        <v>0.266666666666667</v>
       </c>
       <c r="K14">
         <v>47</v>
@@ -5701,14 +5710,14 @@
       <c r="G15">
         <v>70.3</v>
       </c>
-      <c r="H15" s="16">
+      <c r="H15">
         <v>0.31578947368421051</v>
       </c>
       <c r="I15">
         <v>70</v>
       </c>
-      <c r="J15" s="9">
-        <v>0.26315789473684209</v>
+      <c r="J15" s="18">
+        <v>0.26315789473684198</v>
       </c>
       <c r="K15">
         <v>15</v>
@@ -5716,325 +5725,2714 @@
       <c r="N15" s="12"/>
     </row>
     <row r="16" spans="1:14">
-      <c r="D16" s="15" t="s">
+      <c r="G16" s="17"/>
+      <c r="H16" s="16"/>
+      <c r="I16" s="16"/>
+    </row>
+    <row r="17" spans="5:10">
+      <c r="E17" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="F16" s="17" t="s">
+      <c r="F17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>1493</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>1494</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="18" spans="5:10">
+      <c r="E18" s="13" t="s">
+        <v>1479</v>
+      </c>
+      <c r="F18" t="s">
+        <v>5</v>
+      </c>
+      <c r="G18">
+        <v>0.30676691729323308</v>
+      </c>
+      <c r="H18">
+        <v>6.5714285714285712</v>
+      </c>
+      <c r="I18">
+        <v>0.26315789473684198</v>
+      </c>
+      <c r="J18">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="5:10">
+      <c r="E19">
+        <v>0.26315789473684198</v>
+      </c>
+      <c r="F19" t="s">
+        <v>5</v>
+      </c>
+      <c r="G19">
+        <v>0.25152998776009788</v>
+      </c>
+      <c r="H19">
+        <v>6.0348837209302326</v>
+      </c>
+      <c r="I19">
+        <v>0.21052631578947301</v>
+      </c>
+      <c r="J19">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="5:10">
+      <c r="F20" t="s">
+        <v>5</v>
+      </c>
+      <c r="G20">
+        <v>0.2433648223121907</v>
+      </c>
+      <c r="H20">
+        <v>5.817663817663818</v>
+      </c>
+      <c r="I20">
+        <v>0.31578947368421001</v>
+      </c>
+      <c r="J20">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="5:10">
+      <c r="F21" t="s">
+        <v>5</v>
+      </c>
+      <c r="G21">
+        <v>0.2446515290720567</v>
+      </c>
+      <c r="H21">
+        <v>6.0049875311720697</v>
+      </c>
+      <c r="I21">
+        <v>0.42105263157894701</v>
+      </c>
+      <c r="J21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="5:10">
+      <c r="F22" t="s">
+        <v>5</v>
+      </c>
+      <c r="G22">
+        <v>0.25749438531393409</v>
+      </c>
+      <c r="H22">
+        <v>5.8478664192949914</v>
+      </c>
+      <c r="I22">
+        <v>0.31578947368421001</v>
+      </c>
+      <c r="J22">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="5:10">
+      <c r="F23" t="s">
+        <v>5</v>
+      </c>
+      <c r="G23">
+        <v>0.26275115919629061</v>
+      </c>
+      <c r="H23">
+        <v>5.8145285935085012</v>
+      </c>
+      <c r="I23">
+        <v>0.31578947368421001</v>
+      </c>
+      <c r="J23">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="5:10">
+      <c r="F24" t="s">
+        <v>5</v>
+      </c>
+      <c r="G24">
+        <v>0.26984777117892</v>
+      </c>
+      <c r="H24">
+        <v>5.8132295719844356</v>
+      </c>
+      <c r="I24">
+        <v>0.42105263157894701</v>
+      </c>
+      <c r="J24">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="5:10">
+      <c r="F25" t="s">
+        <v>5</v>
+      </c>
+      <c r="G25">
+        <v>0.27713525882862272</v>
+      </c>
+      <c r="H25">
+        <v>5.7555816686251466</v>
+      </c>
+      <c r="I25">
+        <v>0.36842105263157898</v>
+      </c>
+      <c r="J25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="5:10">
+      <c r="F26" t="s">
+        <v>5</v>
+      </c>
+      <c r="G26">
+        <v>0.28229177832565122</v>
+      </c>
+      <c r="H26">
+        <v>5.7708757637474539</v>
+      </c>
+      <c r="I26">
+        <v>0.31578947368421001</v>
+      </c>
+      <c r="J26">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="5:10">
+      <c r="F27" t="s">
+        <v>5</v>
+      </c>
+      <c r="G27">
+        <v>0.27629367536488281</v>
+      </c>
+      <c r="H27">
+        <v>6.1630252100840339</v>
+      </c>
+      <c r="I27">
+        <v>0.31578947368421001</v>
+      </c>
+      <c r="J27">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="5:10">
+      <c r="E28" s="13" t="s">
+        <v>1481</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>1493</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>1494</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="29" spans="5:10">
+      <c r="E29" s="11">
+        <v>9.6774193548387094E-2</v>
+      </c>
+      <c r="F29" t="s">
+        <v>6</v>
+      </c>
+      <c r="G29">
+        <v>7.5268817204301092E-2</v>
+      </c>
+      <c r="H29">
+        <v>17.8</v>
+      </c>
+      <c r="I29">
+        <v>9.6774193548387094E-2</v>
+      </c>
+      <c r="J29">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="5:10">
+      <c r="F30" t="s">
+        <v>6</v>
+      </c>
+      <c r="G30">
+        <v>7.7188940092165911E-2</v>
+      </c>
+      <c r="H30">
+        <v>19.035714285714281</v>
+      </c>
+      <c r="I30" s="12">
+        <v>0.12903225806451599</v>
+      </c>
+      <c r="J30">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="31" spans="5:10">
+      <c r="F31" t="s">
+        <v>6</v>
+      </c>
+      <c r="G31">
+        <v>7.6612903225806467E-2</v>
+      </c>
+      <c r="H31">
+        <v>18.75</v>
+      </c>
+      <c r="I31">
+        <v>3.2258064516128997E-2</v>
+      </c>
+      <c r="J31">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="32" spans="5:10">
+      <c r="F32" t="s">
+        <v>6</v>
+      </c>
+      <c r="G32">
+        <v>7.8784119106699774E-2</v>
+      </c>
+      <c r="H32">
+        <v>18.26923076923077</v>
+      </c>
+      <c r="I32">
+        <v>9.6774193548387094E-2</v>
+      </c>
+      <c r="J32">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="5:10">
+      <c r="F33" t="s">
+        <v>6</v>
+      </c>
+      <c r="G33">
+        <v>7.7515647568608598E-2</v>
+      </c>
+      <c r="H33">
+        <v>18.985074626865671</v>
+      </c>
+      <c r="I33">
+        <v>6.4516129032258104E-2</v>
+      </c>
+      <c r="J33">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="34" spans="5:10">
+      <c r="F34" t="s">
+        <v>6</v>
+      </c>
+      <c r="G34">
+        <v>7.6317859952793096E-2</v>
+      </c>
+      <c r="H34">
+        <v>19.341463414634141</v>
+      </c>
+      <c r="I34">
+        <v>9.6774193548387094E-2</v>
+      </c>
+      <c r="J34">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="35" spans="5:10">
+      <c r="F35" t="s">
+        <v>6</v>
+      </c>
+      <c r="G35">
+        <v>7.6740237691001703E-2</v>
+      </c>
+      <c r="H35">
+        <v>19.578947368421051</v>
+      </c>
+      <c r="I35">
+        <v>9.6774193548387094E-2</v>
+      </c>
+      <c r="J35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36" spans="5:10">
+      <c r="F36" t="s">
+        <v>6</v>
+      </c>
+      <c r="G36">
+        <v>7.7303109561174088E-2</v>
+      </c>
+      <c r="H36">
+        <v>20.027027027027032</v>
+      </c>
+      <c r="I36">
+        <v>6.4516129032258104E-2</v>
+      </c>
+      <c r="J36">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="37" spans="5:10">
+      <c r="F37" t="s">
+        <v>6</v>
+      </c>
+      <c r="G37">
+        <v>7.7620967741935484E-2</v>
+      </c>
+      <c r="H37">
+        <v>19.9375</v>
+      </c>
+      <c r="I37">
+        <v>9.6774193548387094E-2</v>
+      </c>
+      <c r="J37">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="38" spans="5:10">
+      <c r="F38" t="s">
+        <v>6</v>
+      </c>
+      <c r="G38">
+        <v>8.2111436950146624E-2</v>
+      </c>
+      <c r="H38">
+        <v>20.04195804195804</v>
+      </c>
+      <c r="I38">
+        <v>9.6774193548387094E-2</v>
+      </c>
+      <c r="J38">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="39" spans="5:10">
+      <c r="E39" s="13" t="s">
+        <v>1482</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>1493</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>1494</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="40" spans="5:10">
+      <c r="E40">
+        <v>9.0909090909090898E-2</v>
+      </c>
+      <c r="F40" t="s">
+        <v>7</v>
+      </c>
+      <c r="G40">
+        <v>0.12396694214876031</v>
+      </c>
+      <c r="H40">
+        <v>3.1818181818181821</v>
+      </c>
+      <c r="I40">
+        <v>9.0909090909090898E-2</v>
+      </c>
+      <c r="J40">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="5:10">
+      <c r="F41" t="s">
+        <v>7</v>
+      </c>
+      <c r="G41">
+        <v>0.1235795454545455</v>
+      </c>
+      <c r="H41">
+        <v>4.03125</v>
+      </c>
+      <c r="I41">
+        <v>4.54545454545454E-2</v>
+      </c>
+      <c r="J41">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="5:10">
+      <c r="F42" t="s">
+        <v>7</v>
+      </c>
+      <c r="G42">
+        <v>0.13546650717703351</v>
+      </c>
+      <c r="H42">
+        <v>4.0592105263157894</v>
+      </c>
+      <c r="I42">
+        <v>9.0909090909090898E-2</v>
+      </c>
+      <c r="J42">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="5:10">
+      <c r="F43" t="s">
+        <v>7</v>
+      </c>
+      <c r="G43">
+        <v>0.14138623807132089</v>
+      </c>
+      <c r="H43">
+        <v>4.0110497237569058</v>
+      </c>
+      <c r="I43">
+        <v>9.0909090909090898E-2</v>
+      </c>
+      <c r="J43">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="5:10">
+      <c r="F44" t="s">
+        <v>7</v>
+      </c>
+      <c r="G44">
+        <v>0.1357142857142857</v>
+      </c>
+      <c r="H44">
+        <v>4.1619047619047622</v>
+      </c>
+      <c r="I44">
+        <v>0.18181818181818099</v>
+      </c>
+      <c r="J44">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="5:10">
+      <c r="F45" t="s">
+        <v>7</v>
+      </c>
+      <c r="G45">
+        <v>0.14053195712584349</v>
+      </c>
+      <c r="H45">
+        <v>4.1834061135371181</v>
+      </c>
+      <c r="I45">
+        <v>0.13636363636363599</v>
+      </c>
+      <c r="J45">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="5:10">
+      <c r="F46" t="s">
+        <v>7</v>
+      </c>
+      <c r="G46">
+        <v>0.13669301712779969</v>
+      </c>
+      <c r="H46">
+        <v>4.0543478260869561</v>
+      </c>
+      <c r="I46">
+        <v>4.54545454545454E-2</v>
+      </c>
+      <c r="J46">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="5:10">
+      <c r="F47" t="s">
+        <v>7</v>
+      </c>
+      <c r="G47">
+        <v>0.135940146809712</v>
+      </c>
+      <c r="H47">
+        <v>4.0621118012422359</v>
+      </c>
+      <c r="I47">
+        <v>0.13636363636363599</v>
+      </c>
+      <c r="J47">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="5:10">
+      <c r="F48" t="s">
+        <v>7</v>
+      </c>
+      <c r="G48">
+        <v>0.1351981351981352</v>
+      </c>
+      <c r="H48">
+        <v>4.0142450142450139</v>
+      </c>
+      <c r="I48">
+        <v>4.54545454545454E-2</v>
+      </c>
+      <c r="J48">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="5:10">
+      <c r="F49" t="s">
+        <v>7</v>
+      </c>
+      <c r="G49">
+        <v>0.1368590537527867</v>
+      </c>
+      <c r="H49">
+        <v>4.0027247956403267</v>
+      </c>
+      <c r="I49">
+        <v>4.54545454545454E-2</v>
+      </c>
+      <c r="J49">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="5:10">
+      <c r="E50" s="13" t="s">
+        <v>1483</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>1493</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>1494</v>
+      </c>
+      <c r="I50" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="J50" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="51" spans="5:10">
+      <c r="E51">
+        <v>0.27586206896551702</v>
+      </c>
+      <c r="F51" t="s">
+        <v>8</v>
+      </c>
+      <c r="G51">
+        <v>0.30434782608695649</v>
+      </c>
+      <c r="H51">
+        <v>10.956521739130441</v>
+      </c>
+      <c r="I51">
+        <v>0.27586206896551702</v>
+      </c>
+      <c r="J51">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="52" spans="5:10">
+      <c r="F52" t="s">
+        <v>8</v>
+      </c>
+      <c r="G52">
+        <v>0.31034482758620691</v>
+      </c>
+      <c r="H52">
+        <v>9.9534883720930232</v>
+      </c>
+      <c r="I52">
+        <v>0.27586206896551702</v>
+      </c>
+      <c r="J52">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="53" spans="5:10">
+      <c r="F53" t="s">
+        <v>8</v>
+      </c>
+      <c r="G53">
+        <v>0.30441810344827591</v>
+      </c>
+      <c r="H53">
+        <v>10.125</v>
+      </c>
+      <c r="I53">
+        <v>0.27586206896551702</v>
+      </c>
+      <c r="J53">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="54" spans="5:10">
+      <c r="F54" t="s">
+        <v>8</v>
+      </c>
+      <c r="G54">
+        <v>0.30220844633862842</v>
+      </c>
+      <c r="H54">
+        <v>10.20224719101124</v>
+      </c>
+      <c r="I54">
+        <v>0.20689655172413701</v>
+      </c>
+      <c r="J54">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="55" spans="5:10">
+      <c r="F55" t="s">
+        <v>8</v>
+      </c>
+      <c r="G55">
+        <v>0.30308529945553542</v>
+      </c>
+      <c r="H55">
+        <v>11.67543859649123</v>
+      </c>
+      <c r="I55">
+        <v>0.20689655172413701</v>
+      </c>
+      <c r="J55">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="56" spans="5:10">
+      <c r="F56" t="s">
+        <v>8</v>
+      </c>
+      <c r="G56">
+        <v>0.29876847290640401</v>
+      </c>
+      <c r="H56">
+        <v>11.56428571428571</v>
+      </c>
+      <c r="I56">
+        <v>0.20689655172413701</v>
+      </c>
+      <c r="J56">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="57" spans="5:10">
+      <c r="F57" t="s">
+        <v>8</v>
+      </c>
+      <c r="G57">
+        <v>0.29467084639498442</v>
+      </c>
+      <c r="H57">
+        <v>11.62424242424242</v>
+      </c>
+      <c r="I57">
+        <v>0.24137931034482701</v>
+      </c>
+      <c r="J57">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="58" spans="5:10">
+      <c r="F58" t="s">
+        <v>8</v>
+      </c>
+      <c r="G58">
+        <v>0.29274425287356332</v>
+      </c>
+      <c r="H58">
+        <v>11.4375</v>
+      </c>
+      <c r="I58">
+        <v>0.24137931034482701</v>
+      </c>
+      <c r="J58">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="59" spans="5:10">
+      <c r="F59" t="s">
+        <v>8</v>
+      </c>
+      <c r="G59">
+        <v>0.29407025459232999</v>
+      </c>
+      <c r="H59">
+        <v>11.252336448598131</v>
+      </c>
+      <c r="I59">
+        <v>0.31034482758620602</v>
+      </c>
+      <c r="J59">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="60" spans="5:10">
+      <c r="F60" t="s">
+        <v>8</v>
+      </c>
+      <c r="G60">
+        <v>0.29317558793824838</v>
+      </c>
+      <c r="H60">
+        <v>11.20502092050209</v>
+      </c>
+      <c r="I60">
+        <v>0.27586206896551702</v>
+      </c>
+      <c r="J60">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="61" spans="5:10">
+      <c r="E61" s="13" t="s">
+        <v>1484</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>1493</v>
+      </c>
+      <c r="H61" s="1" t="s">
+        <v>1494</v>
+      </c>
+      <c r="I61" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="J61" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="62" spans="5:10">
+      <c r="E62">
+        <v>9.0909090909090898E-2</v>
+      </c>
+      <c r="F62" t="s">
+        <v>10</v>
+      </c>
+      <c r="G62">
+        <v>0.26420454545454553</v>
+      </c>
+      <c r="H62">
+        <v>22.75</v>
+      </c>
+      <c r="I62">
+        <v>0.27272727272727199</v>
+      </c>
+      <c r="J62">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="63" spans="5:10">
+      <c r="F63" t="s">
+        <v>10</v>
+      </c>
+      <c r="G63">
+        <v>0.26175548589341691</v>
+      </c>
+      <c r="H63">
+        <v>20.96551724137931</v>
+      </c>
+      <c r="I63">
+        <v>0.45454545454545398</v>
+      </c>
+      <c r="J63">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="64" spans="5:10">
+      <c r="F64" t="s">
+        <v>10</v>
+      </c>
+      <c r="G64">
+        <v>0.2610993657505285</v>
+      </c>
+      <c r="H64">
+        <v>19.767441860465119</v>
+      </c>
+      <c r="I64">
+        <v>0.45454545454545398</v>
+      </c>
+      <c r="J64">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="65" spans="5:10">
+      <c r="F65" t="s">
+        <v>10</v>
+      </c>
+      <c r="G65">
+        <v>0.25344352617079891</v>
+      </c>
+      <c r="H65">
+        <v>20.166666666666671</v>
+      </c>
+      <c r="I65">
+        <v>0.40909090909090901</v>
+      </c>
+      <c r="J65">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="66" spans="5:10">
+      <c r="F66" t="s">
+        <v>10</v>
+      </c>
+      <c r="G66">
+        <v>0.2600422832980972</v>
+      </c>
+      <c r="H66">
+        <v>20.767441860465119</v>
+      </c>
+      <c r="I66">
+        <v>0.40909090909090901</v>
+      </c>
+      <c r="J66">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="67" spans="5:10">
+      <c r="F67" t="s">
+        <v>10</v>
+      </c>
+      <c r="G67">
+        <v>0.26363636363636361</v>
+      </c>
+      <c r="H67">
+        <v>20.54</v>
+      </c>
+      <c r="I67">
+        <v>0.40909090909090901</v>
+      </c>
+      <c r="J67">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="68" spans="5:10">
+      <c r="F68" t="s">
+        <v>10</v>
+      </c>
+      <c r="G68">
+        <v>0.26961926961926957</v>
+      </c>
+      <c r="H68">
+        <v>21.179487179487179</v>
+      </c>
+      <c r="I68">
+        <v>0.27272727272727199</v>
+      </c>
+      <c r="J68">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="69" spans="5:10">
+      <c r="F69" t="s">
+        <v>10</v>
+      </c>
+      <c r="G69">
+        <v>0.26704545454545459</v>
+      </c>
+      <c r="H69">
+        <v>20.786764705882351</v>
+      </c>
+      <c r="I69">
+        <v>0.31818181818181801</v>
+      </c>
+      <c r="J69">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="70" spans="5:10">
+      <c r="F70" t="s">
+        <v>10</v>
+      </c>
+      <c r="G70">
+        <v>0.26918536009445099</v>
+      </c>
+      <c r="H70">
+        <v>20.487012987012989</v>
+      </c>
+      <c r="I70">
+        <v>0.36363636363636298</v>
+      </c>
+      <c r="J70">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="71" spans="5:10">
+      <c r="F71" t="s">
+        <v>10</v>
+      </c>
+      <c r="G71">
+        <v>0.26546530392684242</v>
+      </c>
+      <c r="H71">
+        <v>20.53254437869823</v>
+      </c>
+      <c r="I71">
+        <v>0.36363636363636298</v>
+      </c>
+      <c r="J71">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="72" spans="5:10">
+      <c r="E72" s="13" t="s">
+        <v>1485</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G72" s="1" t="s">
+        <v>1493</v>
+      </c>
+      <c r="H72" s="1" t="s">
+        <v>1494</v>
+      </c>
+      <c r="I72" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="J72" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="73" spans="5:10">
+      <c r="E73">
+        <v>0.269230769230769</v>
+      </c>
+      <c r="F73" t="s">
+        <v>11</v>
+      </c>
+      <c r="G73">
+        <v>0.24475524475524471</v>
+      </c>
+      <c r="H73">
+        <v>108.59090909090909</v>
+      </c>
+      <c r="I73">
+        <v>0.19230769230769201</v>
+      </c>
+      <c r="J73">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="74" spans="5:10">
+      <c r="F74" t="s">
+        <v>11</v>
+      </c>
+      <c r="G74">
+        <v>0.25404858299595151</v>
+      </c>
+      <c r="H74">
+        <v>107.31578947368421</v>
+      </c>
+      <c r="I74">
+        <v>0.23076923076923</v>
+      </c>
+      <c r="J74">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="75" spans="5:10">
+      <c r="F75" t="s">
+        <v>11</v>
+      </c>
+      <c r="G75">
+        <v>0.23668639053254431</v>
+      </c>
+      <c r="H75">
+        <v>107.4038461538462</v>
+      </c>
+      <c r="I75">
+        <v>0.19230769230769201</v>
+      </c>
+      <c r="J75">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="76" spans="5:10">
+      <c r="F76" t="s">
+        <v>11</v>
+      </c>
+      <c r="G76">
+        <v>0.2395604395604396</v>
+      </c>
+      <c r="H76">
+        <v>106.9</v>
+      </c>
+      <c r="I76">
+        <v>0.269230769230769</v>
+      </c>
+      <c r="J76">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="77" spans="5:10">
+      <c r="F77" t="s">
+        <v>11</v>
+      </c>
+      <c r="G77">
+        <v>0.23509075194468451</v>
+      </c>
+      <c r="H77">
+        <v>107.5168539325843</v>
+      </c>
+      <c r="I77">
+        <v>0.269230769230769</v>
+      </c>
+      <c r="J77">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="78" spans="5:10">
+      <c r="F78" t="s">
+        <v>11</v>
+      </c>
+      <c r="G78">
+        <v>0.23223443223443219</v>
+      </c>
+      <c r="H78">
+        <v>106.84761904761901</v>
+      </c>
+      <c r="I78">
+        <v>0.23076923076923</v>
+      </c>
+      <c r="J78">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="79" spans="5:10">
+      <c r="F79" t="s">
+        <v>11</v>
+      </c>
+      <c r="G79">
+        <v>0.2320406865861411</v>
+      </c>
+      <c r="H79">
+        <v>106.239669421488</v>
+      </c>
+      <c r="I79">
+        <v>0.15384615384615299</v>
+      </c>
+      <c r="J79">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="80" spans="5:10">
+      <c r="F80" t="s">
+        <v>11</v>
+      </c>
+      <c r="G80">
+        <v>0.2342175066312997</v>
+      </c>
+      <c r="H80">
+        <v>107.66206896551719</v>
+      </c>
+      <c r="I80">
+        <v>0.269230769230769</v>
+      </c>
+      <c r="J80">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="81" spans="5:10">
+      <c r="F81" t="s">
+        <v>11</v>
+      </c>
+      <c r="G81">
+        <v>0.23417721518987339</v>
+      </c>
+      <c r="H81">
+        <v>106.7658227848101</v>
+      </c>
+      <c r="I81">
+        <v>0.269230769230769</v>
+      </c>
+      <c r="J81">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="82" spans="5:10">
+      <c r="F82" t="s">
+        <v>11</v>
+      </c>
+      <c r="G82">
+        <v>0.23607427055702909</v>
+      </c>
+      <c r="H82">
+        <v>106.22988505747129</v>
+      </c>
+      <c r="I82">
+        <v>0.23076923076923</v>
+      </c>
+      <c r="J82">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="83" spans="5:10">
+      <c r="E83" s="13" t="s">
+        <v>1486</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G83" s="1" t="s">
+        <v>1493</v>
+      </c>
+      <c r="H83" s="1" t="s">
+        <v>1494</v>
+      </c>
+      <c r="I83" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="J83" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="84" spans="5:10">
+      <c r="E84">
+        <v>4.91803278688525E-2</v>
+      </c>
+      <c r="F84" t="s">
+        <v>12</v>
+      </c>
+      <c r="G84">
+        <v>0.1209016393442623</v>
+      </c>
+      <c r="H84">
+        <v>7</v>
+      </c>
+      <c r="I84">
+        <v>0.14754098360655701</v>
+      </c>
+      <c r="J84">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="85" spans="5:10">
+      <c r="F85" t="s">
+        <v>12</v>
+      </c>
+      <c r="G85">
+        <v>9.8360655737704916E-2</v>
+      </c>
+      <c r="H85">
+        <v>6.2236842105263159</v>
+      </c>
+      <c r="I85">
+        <v>8.1967213114753995E-2</v>
+      </c>
+      <c r="J85">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="86" spans="5:10">
+      <c r="F86" t="s">
+        <v>12</v>
+      </c>
+      <c r="G86">
+        <v>0.1040552200172563</v>
+      </c>
+      <c r="H86">
+        <v>6.0842105263157897</v>
+      </c>
+      <c r="I86">
+        <v>8.1967213114753995E-2</v>
+      </c>
+      <c r="J86">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="87" spans="5:10">
+      <c r="F87" t="s">
+        <v>12</v>
+      </c>
+      <c r="G87">
+        <v>9.6004711887699989E-2</v>
+      </c>
+      <c r="H87">
+        <v>6.3053892215568874</v>
+      </c>
+      <c r="I87">
+        <v>6.5573770491803199E-2</v>
+      </c>
+      <c r="J87">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="88" spans="5:10">
+      <c r="F88" t="s">
+        <v>12</v>
+      </c>
+      <c r="G88">
+        <v>9.6699646132736322E-2</v>
+      </c>
+      <c r="H88">
+        <v>6.3876651982378858</v>
+      </c>
+      <c r="I88">
+        <v>8.1967213114753995E-2</v>
+      </c>
+      <c r="J88">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="89" spans="5:10">
+      <c r="F89" t="s">
+        <v>12</v>
+      </c>
+      <c r="G89">
+        <v>9.7897236864971329E-2</v>
+      </c>
+      <c r="H89">
+        <v>6.6501766784452299</v>
+      </c>
+      <c r="I89">
+        <v>6.5573770491803199E-2</v>
+      </c>
+      <c r="J89">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="90" spans="5:10">
+      <c r="F90" t="s">
+        <v>12</v>
+      </c>
+      <c r="G90">
+        <v>0.10158890290037829</v>
+      </c>
+      <c r="H90">
+        <v>6.5353846153846158</v>
+      </c>
+      <c r="I90">
+        <v>0.13114754098360601</v>
+      </c>
+      <c r="J90">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="91" spans="5:10">
+      <c r="F91" t="s">
+        <v>12</v>
+      </c>
+      <c r="G91">
+        <v>0.1018964963034394</v>
+      </c>
+      <c r="H91">
+        <v>6.6414565826330536</v>
+      </c>
+      <c r="I91">
+        <v>9.8360655737704902E-2</v>
+      </c>
+      <c r="J91">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="92" spans="5:10">
+      <c r="F92" t="s">
+        <v>12</v>
+      </c>
+      <c r="G92">
+        <v>0.1027924788090013</v>
+      </c>
+      <c r="H92">
+        <v>6.650918635170604</v>
+      </c>
+      <c r="I92">
+        <v>0.16393442622950799</v>
+      </c>
+      <c r="J92">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="93" spans="5:10">
+      <c r="F93" t="s">
+        <v>12</v>
+      </c>
+      <c r="G93">
+        <v>0.102576112412178</v>
+      </c>
+      <c r="H93">
+        <v>6.6071428571428568</v>
+      </c>
+      <c r="I93">
+        <v>0.13114754098360601</v>
+      </c>
+      <c r="J93">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="94" spans="5:10">
+      <c r="E94" s="13" t="s">
+        <v>1487</v>
+      </c>
+      <c r="F94" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G94" s="1" t="s">
+        <v>1493</v>
+      </c>
+      <c r="H94" s="1" t="s">
+        <v>1494</v>
+      </c>
+      <c r="I94" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="J94" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="95" spans="5:10">
+      <c r="E95">
+        <v>0.19999999999999599</v>
+      </c>
+      <c r="F95" t="s">
+        <v>13</v>
+      </c>
+      <c r="G95">
+        <v>0.3396825396825397</v>
+      </c>
+      <c r="H95">
+        <v>20.095238095238091</v>
+      </c>
+      <c r="I95">
+        <v>0.4</v>
+      </c>
+      <c r="J95">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="96" spans="5:10">
+      <c r="F96" t="s">
+        <v>13</v>
+      </c>
+      <c r="G96">
+        <v>0.33921568627450988</v>
+      </c>
+      <c r="H96">
+        <v>19.235294117647062</v>
+      </c>
+      <c r="I96">
+        <v>0.53333333333333299</v>
+      </c>
+      <c r="J96">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="97" spans="5:10">
+      <c r="F97" t="s">
+        <v>13</v>
+      </c>
+      <c r="G97">
+        <v>0.33856209150326788</v>
+      </c>
+      <c r="H97">
+        <v>18.901960784313729</v>
+      </c>
+      <c r="I97">
+        <v>0.19999999999999901</v>
+      </c>
+      <c r="J97">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="98" spans="5:10">
+      <c r="F98" t="s">
+        <v>13</v>
+      </c>
+      <c r="G98">
+        <v>0.34476190476190471</v>
+      </c>
+      <c r="H98">
+        <v>19.285714285714281</v>
+      </c>
+      <c r="I98">
+        <v>0.66666666666666596</v>
+      </c>
+      <c r="J98">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="99" spans="5:10">
+      <c r="F99" t="s">
+        <v>13</v>
+      </c>
+      <c r="G99">
+        <v>0.3547892720306513</v>
+      </c>
+      <c r="H99">
+        <v>20.03448275862069</v>
+      </c>
+      <c r="I99">
+        <v>0.46666666666666601</v>
+      </c>
+      <c r="J99">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="100" spans="5:10">
+      <c r="F100" t="s">
+        <v>13</v>
+      </c>
+      <c r="G100">
+        <v>0.35246913580246919</v>
+      </c>
+      <c r="H100">
+        <v>21.444444444444439</v>
+      </c>
+      <c r="I100">
+        <v>0.53333333333333299</v>
+      </c>
+      <c r="J100">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="101" spans="5:10">
+      <c r="F101" t="s">
+        <v>13</v>
+      </c>
+      <c r="G101">
+        <v>0.35609756097560979</v>
+      </c>
+      <c r="H101">
+        <v>21.609756097560979</v>
+      </c>
+      <c r="I101">
+        <v>0.46666666666666601</v>
+      </c>
+      <c r="J101">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="102" spans="5:10">
+      <c r="F102" t="s">
+        <v>13</v>
+      </c>
+      <c r="G102">
+        <v>0.35142857142857142</v>
+      </c>
+      <c r="H102">
+        <v>21.45</v>
+      </c>
+      <c r="I102">
+        <v>0.266666666666666</v>
+      </c>
+      <c r="J102">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="103" spans="5:10">
+      <c r="F103" t="s">
+        <v>13</v>
+      </c>
+      <c r="G103">
+        <v>0.34236559139784939</v>
+      </c>
+      <c r="H103">
+        <v>21.258064516129028</v>
+      </c>
+      <c r="I103">
+        <v>6.6666666666666596E-2</v>
+      </c>
+      <c r="J103">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="104" spans="5:10">
+      <c r="F104" t="s">
+        <v>13</v>
+      </c>
+      <c r="G104">
+        <v>0.34263565891472869</v>
+      </c>
+      <c r="H104">
+        <v>20.93023255813954</v>
+      </c>
+      <c r="I104">
+        <v>0.4</v>
+      </c>
+      <c r="J104">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="105" spans="5:10">
+      <c r="E105" s="13" t="s">
         <v>1488</v>
       </c>
-      <c r="G16" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="H16" s="18" t="s">
+      <c r="F105" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G105" s="1" t="s">
+        <v>1493</v>
+      </c>
+      <c r="H105" s="1" t="s">
+        <v>1494</v>
+      </c>
+      <c r="I105" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="I16" s="18" t="s">
+      <c r="J105" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="17" spans="4:9">
-      <c r="D17">
+    <row r="106" spans="5:10">
+      <c r="E106">
+        <v>0.47058823529411697</v>
+      </c>
+      <c r="F106" t="s">
+        <v>1495</v>
+      </c>
+      <c r="G106">
+        <v>0.48039215686274511</v>
+      </c>
+      <c r="H106">
+        <v>63.571428571428569</v>
+      </c>
+      <c r="I106">
+        <v>0.47058823529411697</v>
+      </c>
+      <c r="J106">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="107" spans="5:10">
+      <c r="F107" t="s">
+        <v>1495</v>
+      </c>
+      <c r="G107">
+        <v>0.46101231190150471</v>
+      </c>
+      <c r="H107">
+        <v>64.465116279069761</v>
+      </c>
+      <c r="I107">
+        <v>0.52941176470588203</v>
+      </c>
+      <c r="J107">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="108" spans="5:10">
+      <c r="F108" t="s">
+        <v>1495</v>
+      </c>
+      <c r="G108">
+        <v>0.44537815126050412</v>
+      </c>
+      <c r="H108">
+        <v>58.971428571428568</v>
+      </c>
+      <c r="I108">
+        <v>0.47058823529411697</v>
+      </c>
+      <c r="J108">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="109" spans="5:10">
+      <c r="F109" t="s">
+        <v>1495</v>
+      </c>
+      <c r="G109">
+        <v>0.44183006535947711</v>
+      </c>
+      <c r="H109">
+        <v>60.533333333333331</v>
+      </c>
+      <c r="I109">
+        <v>0.55882352941176405</v>
+      </c>
+      <c r="J109">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="110" spans="5:10">
+      <c r="F110" t="s">
+        <v>1495</v>
+      </c>
+      <c r="G110">
+        <v>0.43508214096449388</v>
+      </c>
+      <c r="H110">
+        <v>59.18018018018018</v>
+      </c>
+      <c r="I110">
+        <v>0.41176470588235198</v>
+      </c>
+      <c r="J110">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="111" spans="5:10">
+      <c r="F111" t="s">
+        <v>1495</v>
+      </c>
+      <c r="G111">
+        <v>0.43415276558384552</v>
+      </c>
+      <c r="H111">
+        <v>59.305970149253731</v>
+      </c>
+      <c r="I111">
+        <v>0.52941176470588203</v>
+      </c>
+      <c r="J111">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="112" spans="5:10">
+      <c r="F112" t="s">
+        <v>1495</v>
+      </c>
+      <c r="G112">
+        <v>0.42952275249722521</v>
+      </c>
+      <c r="H112">
+        <v>59.459119496855337</v>
+      </c>
+      <c r="I112">
+        <v>0.5</v>
+      </c>
+      <c r="J112">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="113" spans="5:10">
+      <c r="F113" t="s">
+        <v>1495</v>
+      </c>
+      <c r="G113">
+        <v>0.42762723066754788</v>
+      </c>
+      <c r="H113">
+        <v>59.719101123595507</v>
+      </c>
+      <c r="I113">
+        <v>0.52941176470588203</v>
+      </c>
+      <c r="J113">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="114" spans="5:10">
+      <c r="F114" t="s">
+        <v>1495</v>
+      </c>
+      <c r="G114">
+        <v>0.43057629143027759</v>
+      </c>
+      <c r="H114">
+        <v>58.751269035532992</v>
+      </c>
+      <c r="I114">
+        <v>0.41176470588235198</v>
+      </c>
+      <c r="J114">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="115" spans="5:10">
+      <c r="F115" t="s">
+        <v>1495</v>
+      </c>
+      <c r="G115">
+        <v>0.42818057455540359</v>
+      </c>
+      <c r="H115">
+        <v>60.33953488372093</v>
+      </c>
+      <c r="I115">
+        <v>0.47058823529411697</v>
+      </c>
+      <c r="J115">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="116" spans="5:10">
+      <c r="E116" s="13" t="s">
+        <v>1489</v>
+      </c>
+      <c r="F116" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G116" s="1" t="s">
+        <v>1493</v>
+      </c>
+      <c r="H116" s="1" t="s">
+        <v>1494</v>
+      </c>
+      <c r="I116" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="J116" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="117" spans="5:10">
+      <c r="E117">
+        <v>0.25862068965517199</v>
+      </c>
+      <c r="F117" t="s">
+        <v>832</v>
+      </c>
+      <c r="G117">
+        <v>0.31773399014778331</v>
+      </c>
+      <c r="H117">
+        <v>77.607142857142861</v>
+      </c>
+      <c r="I117">
+        <v>0.39655172413793099</v>
+      </c>
+      <c r="J117">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="118" spans="5:10">
+      <c r="F118" t="s">
+        <v>832</v>
+      </c>
+      <c r="G118">
+        <v>0.31458451102317703</v>
+      </c>
+      <c r="H118">
+        <v>79.540983606557376</v>
+      </c>
+      <c r="I118">
+        <v>0.39655172413793099</v>
+      </c>
+      <c r="J118">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="119" spans="5:10">
+      <c r="F119" t="s">
+        <v>832</v>
+      </c>
+      <c r="G119">
+        <v>0.31465517241379309</v>
+      </c>
+      <c r="H119">
+        <v>82.034090909090907</v>
+      </c>
+      <c r="I119">
+        <v>0.37931034482758602</v>
+      </c>
+      <c r="J119">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="120" spans="5:10">
+      <c r="F120" t="s">
+        <v>832</v>
+      </c>
+      <c r="G120">
+        <v>0.31859711170055988</v>
+      </c>
+      <c r="H120">
+        <v>82.384615384615387</v>
+      </c>
+      <c r="I120">
+        <v>0.37931034482758602</v>
+      </c>
+      <c r="J120">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="121" spans="5:10">
+      <c r="F121" t="s">
+        <v>832</v>
+      </c>
+      <c r="G121">
+        <v>0.32342871117632682</v>
+      </c>
+      <c r="H121">
+        <v>80.765957446808514</v>
+      </c>
+      <c r="I121">
+        <v>0.34482758620689602</v>
+      </c>
+      <c r="J121">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="122" spans="5:10">
+      <c r="F122" t="s">
+        <v>832</v>
+      </c>
+      <c r="G122">
+        <v>0.32299530708018759</v>
+      </c>
+      <c r="H122">
+        <v>82.301775147928993</v>
+      </c>
+      <c r="I122">
+        <v>0.36206896551724099</v>
+      </c>
+      <c r="J122">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="123" spans="5:10">
+      <c r="F123" t="s">
+        <v>832</v>
+      </c>
+      <c r="G123">
+        <v>0.32218219248584662</v>
+      </c>
+      <c r="H123">
+        <v>82.184079601990049</v>
+      </c>
+      <c r="I123">
+        <v>0.37931034482758602</v>
+      </c>
+      <c r="J123">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="124" spans="5:10">
+      <c r="F124" t="s">
+        <v>832</v>
+      </c>
+      <c r="G124">
+        <v>0.32300884955752213</v>
+      </c>
+      <c r="H124">
+        <v>81.579646017699119</v>
+      </c>
+      <c r="I124">
+        <v>0.37931034482758602</v>
+      </c>
+      <c r="J124">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="125" spans="5:10">
+      <c r="F125" t="s">
+        <v>832</v>
+      </c>
+      <c r="G125">
+        <v>0.32341056034482762</v>
+      </c>
+      <c r="H125">
+        <v>80.01171875</v>
+      </c>
+      <c r="I125">
+        <v>0.34482758620689602</v>
+      </c>
+      <c r="J125">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="126" spans="5:10">
+      <c r="F126" t="s">
+        <v>832</v>
+      </c>
+      <c r="G126">
+        <v>0.32240173619483958</v>
+      </c>
+      <c r="H126">
+        <v>80.52447552447552</v>
+      </c>
+      <c r="I126">
+        <v>0.37931034482758602</v>
+      </c>
+      <c r="J126">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="127" spans="5:10">
+      <c r="E127" s="13" t="s">
+        <v>1490</v>
+      </c>
+      <c r="F127" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G127" s="1" t="s">
+        <v>1493</v>
+      </c>
+      <c r="H127" s="1" t="s">
+        <v>1494</v>
+      </c>
+      <c r="I127" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="J127" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="128" spans="5:10">
+      <c r="E128">
+        <v>0.11111111111111099</v>
+      </c>
+      <c r="F128" t="s">
+        <v>1496</v>
+      </c>
+      <c r="G128">
+        <v>9.3121693121693133E-2</v>
+      </c>
+      <c r="H128">
+        <v>5.7523809523809524</v>
+      </c>
+      <c r="I128">
+        <v>7.4074074074074001E-2</v>
+      </c>
+      <c r="J128">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="129" spans="5:10">
+      <c r="F129" t="s">
+        <v>1496</v>
+      </c>
+      <c r="G129">
+        <v>8.9163237311385493E-2</v>
+      </c>
+      <c r="H129">
+        <v>5.9576719576719572</v>
+      </c>
+      <c r="I129">
+        <v>3.7037037037037E-2</v>
+      </c>
+      <c r="J129">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="130" spans="5:10">
+      <c r="F130" t="s">
+        <v>1496</v>
+      </c>
+      <c r="G130">
+        <v>0.11578455427035871</v>
+      </c>
+      <c r="H130">
+        <v>5.7192429022082019</v>
+      </c>
+      <c r="I130">
+        <v>0.18518518518518501</v>
+      </c>
+      <c r="J130">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="131" spans="5:10">
+      <c r="F131" t="s">
+        <v>1496</v>
+      </c>
+      <c r="G131">
+        <v>0.12585733882030181</v>
+      </c>
+      <c r="H131">
+        <v>5.666666666666667</v>
+      </c>
+      <c r="I131">
+        <v>0.11111111111111099</v>
+      </c>
+      <c r="J131">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="132" spans="5:10">
+      <c r="F132" t="s">
+        <v>1496</v>
+      </c>
+      <c r="G132">
+        <v>0.12066240637669209</v>
+      </c>
+      <c r="H132">
+        <v>5.7217068645640072</v>
+      </c>
+      <c r="I132">
+        <v>7.4074074074074001E-2</v>
+      </c>
+      <c r="J132">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="133" spans="5:10">
+      <c r="F133" t="s">
+        <v>1496</v>
+      </c>
+      <c r="G133">
+        <v>0.11759849020995521</v>
+      </c>
+      <c r="H133">
+        <v>5.7993630573248396</v>
+      </c>
+      <c r="I133">
+        <v>0.148148148148148</v>
+      </c>
+      <c r="J133">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="134" spans="5:10">
+      <c r="F134" t="s">
+        <v>1496</v>
+      </c>
+      <c r="G134">
+        <v>0.12120308227690781</v>
+      </c>
+      <c r="H134">
+        <v>5.8174496644295299</v>
+      </c>
+      <c r="I134">
+        <v>0.148148148148148</v>
+      </c>
+      <c r="J134">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="135" spans="5:10">
+      <c r="F135" t="s">
+        <v>1496</v>
+      </c>
+      <c r="G135">
+        <v>0.1210433491135246</v>
+      </c>
+      <c r="H135">
+        <v>5.825814536340852</v>
+      </c>
+      <c r="I135">
+        <v>0.11111111111111099</v>
+      </c>
+      <c r="J135">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="136" spans="5:10">
+      <c r="F136" t="s">
+        <v>1496</v>
+      </c>
+      <c r="G136">
+        <v>0.1223043346730628</v>
+      </c>
+      <c r="H136">
+        <v>5.7946324387397903</v>
+      </c>
+      <c r="I136">
+        <v>0.11111111111111099</v>
+      </c>
+      <c r="J136">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="137" spans="5:10">
+      <c r="F137" t="s">
+        <v>1496</v>
+      </c>
+      <c r="G137">
+        <v>0.12069672895453359</v>
+      </c>
+      <c r="H137">
+        <v>5.7985901309164154</v>
+      </c>
+      <c r="I137">
+        <v>3.7037037037037E-2</v>
+      </c>
+      <c r="J137">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="138" spans="5:10">
+      <c r="E138" s="13" t="s">
+        <v>1491</v>
+      </c>
+      <c r="F138" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G138" s="1" t="s">
+        <v>1493</v>
+      </c>
+      <c r="H138" s="1" t="s">
+        <v>1494</v>
+      </c>
+      <c r="I138" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="J138" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="139" spans="5:10">
+      <c r="E139">
+        <v>0.20689655172413701</v>
+      </c>
+      <c r="F139" t="s">
+        <v>1060</v>
+      </c>
+      <c r="G139">
+        <v>0.25412293853073459</v>
+      </c>
+      <c r="H139">
+        <v>171.56521739130429</v>
+      </c>
+      <c r="I139">
+        <v>0.27586206896551702</v>
+      </c>
+      <c r="J139">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="140" spans="5:10">
+      <c r="F140" t="s">
+        <v>1060</v>
+      </c>
+      <c r="G140">
+        <v>0.25143678160919541</v>
+      </c>
+      <c r="H140">
+        <v>171.83333333333329</v>
+      </c>
+      <c r="I140">
+        <v>0.27586206896551702</v>
+      </c>
+      <c r="J140">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="141" spans="5:10">
+      <c r="F141" t="s">
+        <v>1060</v>
+      </c>
+      <c r="G141">
+        <v>0.2459291187739463</v>
+      </c>
+      <c r="H141">
+        <v>176.2222222222222</v>
+      </c>
+      <c r="I141">
+        <v>0.32758620689655099</v>
+      </c>
+      <c r="J141">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="142" spans="5:10">
+      <c r="F142" t="s">
+        <v>1060</v>
+      </c>
+      <c r="G142">
+        <v>0.2473005921281784</v>
+      </c>
+      <c r="H142">
+        <v>176.57575757575759</v>
+      </c>
+      <c r="I142">
+        <v>0.32758620689655099</v>
+      </c>
+      <c r="J142">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="143" spans="5:10">
+      <c r="F143" t="s">
+        <v>1060</v>
+      </c>
+      <c r="G143">
+        <v>0.2438229704045615</v>
+      </c>
+      <c r="H143">
+        <v>178.25984251968501</v>
+      </c>
+      <c r="I143">
+        <v>0.20689655172413701</v>
+      </c>
+      <c r="J143">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="144" spans="5:10">
+      <c r="F144" t="s">
+        <v>1060</v>
+      </c>
+      <c r="G144">
+        <v>0.24257965953731991</v>
+      </c>
+      <c r="H144">
+        <v>178.58860759493669</v>
+      </c>
+      <c r="I144">
+        <v>0.20689655172413701</v>
+      </c>
+      <c r="J144">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="145" spans="5:10">
+      <c r="F145" t="s">
+        <v>1060</v>
+      </c>
+      <c r="G145">
+        <v>0.24471635150166851</v>
+      </c>
+      <c r="H145">
+        <v>177.80107526881719</v>
+      </c>
+      <c r="I145">
+        <v>0.25862068965517199</v>
+      </c>
+      <c r="J145">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="146" spans="5:10">
+      <c r="F146" t="s">
+        <v>1060</v>
+      </c>
+      <c r="G146">
+        <v>0.24398178269355891</v>
+      </c>
+      <c r="H146">
+        <v>176.9858490566038</v>
+      </c>
+      <c r="I146">
+        <v>0.31034482758620602</v>
+      </c>
+      <c r="J146">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="147" spans="5:10">
+      <c r="F147" t="s">
+        <v>1060</v>
+      </c>
+      <c r="G147">
+        <v>0.24524375743162899</v>
+      </c>
+      <c r="H147">
+        <v>176.33620689655169</v>
+      </c>
+      <c r="I147">
+        <v>0.32758620689655099</v>
+      </c>
+      <c r="J147">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="148" spans="5:10">
+      <c r="F148" t="s">
+        <v>1060</v>
+      </c>
+      <c r="G148">
+        <v>0.24575700431034481</v>
+      </c>
+      <c r="H148">
+        <v>176.328125</v>
+      </c>
+      <c r="I148">
+        <v>0.32758620689655099</v>
+      </c>
+      <c r="J148">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="149" spans="5:10">
+      <c r="E149" s="13" t="s">
+        <v>1492</v>
+      </c>
+      <c r="F149" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G149" s="1" t="s">
+        <v>1493</v>
+      </c>
+      <c r="H149" s="1" t="s">
+        <v>1494</v>
+      </c>
+      <c r="I149" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="J149" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="150" spans="5:10">
+      <c r="E150">
+        <v>0.36666666666666597</v>
+      </c>
+      <c r="F150" t="s">
+        <v>1268</v>
+      </c>
+      <c r="G150">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H150">
+        <v>1373.45</v>
+      </c>
+      <c r="I150">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="J150">
+        <v>1373</v>
+      </c>
+    </row>
+    <row r="151" spans="5:10">
+      <c r="F151" t="s">
+        <v>1268</v>
+      </c>
+      <c r="G151">
+        <v>0.33513513513513532</v>
+      </c>
+      <c r="H151">
+        <v>1350.1891891891889</v>
+      </c>
+      <c r="I151">
+        <v>0.3</v>
+      </c>
+      <c r="J151">
+        <v>1350</v>
+      </c>
+    </row>
+    <row r="152" spans="5:10">
+      <c r="F152" t="s">
+        <v>1268</v>
+      </c>
+      <c r="G152">
+        <v>0.33137254901960789</v>
+      </c>
+      <c r="H152">
+        <v>1338.35294117647</v>
+      </c>
+      <c r="I152">
+        <v>0.3</v>
+      </c>
+      <c r="J152">
+        <v>1338</v>
+      </c>
+    </row>
+    <row r="153" spans="5:10">
+      <c r="F153" t="s">
+        <v>1268</v>
+      </c>
+      <c r="G153">
+        <v>0.33582089552238809</v>
+      </c>
+      <c r="H153">
+        <v>1329.268656716418</v>
+      </c>
+      <c r="I153">
+        <v>0.3</v>
+      </c>
+      <c r="J153">
+        <v>1329</v>
+      </c>
+    </row>
+    <row r="154" spans="5:10">
+      <c r="F154" t="s">
+        <v>1268</v>
+      </c>
+      <c r="G154">
+        <v>0.33493975903614459</v>
+      </c>
+      <c r="H154">
+        <v>1324.5783132530121</v>
+      </c>
+      <c r="I154">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="J154">
+        <v>1324</v>
+      </c>
+    </row>
+    <row r="155" spans="5:10">
+      <c r="F155" t="s">
+        <v>1268</v>
+      </c>
+      <c r="G155">
+        <v>0.33775510204081632</v>
+      </c>
+      <c r="H155">
+        <v>1319.6428571428571</v>
+      </c>
+      <c r="I155">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="J155">
+        <v>1319</v>
+      </c>
+    </row>
+    <row r="156" spans="5:10">
+      <c r="F156" t="s">
+        <v>1268</v>
+      </c>
+      <c r="G156">
+        <v>0.33918128654970758</v>
+      </c>
+      <c r="H156">
+        <v>1321.5526315789471</v>
+      </c>
+      <c r="I156">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="J156">
+        <v>1321</v>
+      </c>
+    </row>
+    <row r="157" spans="5:10">
+      <c r="F157" t="s">
+        <v>1268</v>
+      </c>
+      <c r="G157">
+        <v>0.33564102564102571</v>
+      </c>
+      <c r="H157">
+        <v>1320.646153846154</v>
+      </c>
+      <c r="I157">
+        <v>0.266666666666666</v>
+      </c>
+      <c r="J157">
+        <v>1320</v>
+      </c>
+    </row>
+    <row r="158" spans="5:10">
+      <c r="F158" t="s">
+        <v>1268</v>
+      </c>
+      <c r="G158">
+        <v>0.3376712328767123</v>
+      </c>
+      <c r="H158">
+        <v>1318.321917808219</v>
+      </c>
+      <c r="I158">
+        <v>0.3</v>
+      </c>
+      <c r="J158">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="159" spans="5:10">
+      <c r="F159" t="s">
+        <v>1268</v>
+      </c>
+      <c r="G159">
+        <v>0.33926380368098169</v>
+      </c>
+      <c r="H159">
+        <v>1319.423312883436</v>
+      </c>
+      <c r="I159">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="J159">
+        <v>1319</v>
+      </c>
+    </row>
+    <row r="160" spans="5:10">
+      <c r="E160" s="13" t="s">
+        <v>1478</v>
+      </c>
+      <c r="F160" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G160" s="1" t="s">
+        <v>1493</v>
+      </c>
+      <c r="H160" s="1" t="s">
+        <v>1494</v>
+      </c>
+      <c r="I160" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="J160" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="161" spans="5:10">
+      <c r="E161">
         <v>0.26315789473684198</v>
       </c>
-      <c r="E17" s="13" t="s">
-        <v>1479</v>
-      </c>
-      <c r="F17" s="9">
-        <v>0.25882521082065058</v>
-      </c>
-      <c r="G17">
-        <v>6.2322637940473351</v>
-      </c>
-      <c r="H17" s="16">
+      <c r="F161" t="s">
+        <v>1372</v>
+      </c>
+      <c r="G161">
+        <v>0.35789473684210532</v>
+      </c>
+      <c r="H161">
+        <v>75.8</v>
+      </c>
+      <c r="I161">
         <v>0.26315789473684198</v>
       </c>
-      <c r="I17">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="4:9">
-      <c r="D18" s="11">
-        <v>9.6774193548387094E-2</v>
-      </c>
-      <c r="E18" s="13" t="s">
-        <v>1481</v>
-      </c>
-      <c r="F18">
-        <v>7.8925199355529344E-2</v>
-      </c>
-      <c r="G18">
-        <v>20.119241993598521</v>
-      </c>
-      <c r="H18" s="9">
-        <v>6.4516129032258104E-2</v>
-      </c>
-      <c r="I18">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="4:9">
-      <c r="D19" s="9">
-        <v>9.0909090909090898E-2</v>
-      </c>
-      <c r="E19" s="13" t="s">
-        <v>1482</v>
-      </c>
-      <c r="F19">
-        <v>0.139644334868811</v>
-      </c>
-      <c r="G19">
-        <v>4.2859637205471897</v>
-      </c>
-      <c r="H19" s="16">
-        <v>0.13636363636363599</v>
-      </c>
-      <c r="I19">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="4:9">
-      <c r="D20">
-        <v>0.27586206896551702</v>
-      </c>
-      <c r="E20" s="13" t="s">
-        <v>1483</v>
-      </c>
-      <c r="F20">
-        <v>0.26277888543004002</v>
-      </c>
-      <c r="G20">
-        <v>13.4902947984354</v>
-      </c>
-      <c r="H20" s="9">
-        <v>0.24137931034482701</v>
-      </c>
-      <c r="I20">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="21" spans="4:9">
-      <c r="D21" s="9">
-        <v>9.0909090909090898E-2</v>
-      </c>
-      <c r="E21" s="13" t="s">
-        <v>1484</v>
-      </c>
-      <c r="F21">
-        <v>0.24651068245259899</v>
-      </c>
-      <c r="G21">
-        <v>21.302000965436299</v>
-      </c>
-      <c r="H21" s="16">
-        <v>0.31818181818181801</v>
-      </c>
-      <c r="I21">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="4:9">
-      <c r="D22">
-        <v>0.269230769230769</v>
-      </c>
-      <c r="E22" s="13" t="s">
-        <v>1485</v>
-      </c>
-      <c r="F22" s="9">
-        <v>0.22423249336415199</v>
-      </c>
-      <c r="G22">
-        <v>107.23197567746099</v>
-      </c>
-      <c r="H22" s="16">
-        <v>0.23076923076923</v>
-      </c>
-      <c r="I22">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="23" spans="4:9">
-      <c r="D23" s="9">
-        <v>4.91803278688525E-2</v>
-      </c>
-      <c r="E23" s="13" t="s">
-        <v>1486</v>
-      </c>
-      <c r="F23">
-        <v>7.9877338019228999E-2</v>
-      </c>
-      <c r="G23">
-        <v>6.1696984593474804</v>
-      </c>
-      <c r="H23" s="16">
-        <v>0.13114754098360601</v>
-      </c>
-      <c r="I23">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="4:9">
-      <c r="D24" s="9">
-        <v>0.19999999999999599</v>
-      </c>
-      <c r="E24" s="13" t="s">
-        <v>1487</v>
-      </c>
-      <c r="F24" s="16">
-        <v>0.34254998395679398</v>
-      </c>
-      <c r="G24">
-        <v>21.681862659058901</v>
-      </c>
-      <c r="H24" s="16">
-        <v>0.4</v>
-      </c>
-      <c r="I24" s="16">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="25" spans="4:9">
-      <c r="D25">
-        <v>0.47058823529411697</v>
-      </c>
-      <c r="E25" s="13" t="s">
-        <v>1489</v>
-      </c>
-      <c r="F25" s="9">
-        <v>0.41275721182673702</v>
-      </c>
-      <c r="G25">
-        <v>63.9374573165057</v>
-      </c>
-      <c r="H25" s="16">
-        <v>0.52941176470588203</v>
-      </c>
-      <c r="I25" s="16">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="26" spans="4:9">
-      <c r="D26" s="9">
-        <v>0.25862068965517199</v>
-      </c>
-      <c r="E26" s="13" t="s">
-        <v>1490</v>
-      </c>
-      <c r="F26" s="16">
-        <v>0.27070697715380099</v>
-      </c>
-      <c r="G26">
-        <v>101.363239664516</v>
-      </c>
-      <c r="H26" s="16">
-        <v>0.32758620689655099</v>
-      </c>
-      <c r="I26" s="16">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="27" spans="4:9">
-      <c r="D27" s="16">
-        <v>0.11111111111111099</v>
-      </c>
-      <c r="E27" s="13" t="s">
-        <v>1491</v>
-      </c>
-      <c r="F27" s="16">
-        <v>0.11533844328058</v>
-      </c>
-      <c r="G27">
-        <v>5.8628323650880896</v>
-      </c>
-      <c r="H27" s="9">
-        <v>7.4074074074074001E-2</v>
-      </c>
-      <c r="I27" s="16">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="28" spans="4:9">
-      <c r="D28" s="16">
-        <v>0.20689655172413701</v>
-      </c>
-      <c r="E28" s="13" t="s">
-        <v>1492</v>
-      </c>
-      <c r="F28" s="16">
-        <v>0.22977282397554499</v>
-      </c>
-      <c r="G28">
-        <v>196.07003756648501</v>
-      </c>
-      <c r="H28" s="9">
-        <v>0.18965517241379301</v>
-      </c>
-      <c r="I28" s="16">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="29" spans="4:9">
-      <c r="D29">
-        <v>0.36666666666666597</v>
-      </c>
-      <c r="E29" s="13" t="s">
-        <v>1493</v>
-      </c>
-      <c r="F29" s="16">
-        <v>0.334694887027635</v>
-      </c>
-      <c r="G29">
-        <v>1349.97021000167</v>
-      </c>
-      <c r="H29" s="9">
-        <v>0.266666666666666</v>
-      </c>
-      <c r="I29" s="16">
-        <v>1350</v>
-      </c>
-    </row>
-    <row r="30" spans="4:9">
-      <c r="D30">
-        <v>0.26315789473684198</v>
-      </c>
-      <c r="E30" s="13" t="s">
-        <v>1478</v>
-      </c>
-      <c r="F30">
-        <v>0.37873912744386379</v>
-      </c>
-      <c r="G30">
-        <v>75.913257701386712</v>
-      </c>
-      <c r="H30">
+      <c r="J161">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="162" spans="5:10">
+      <c r="F162" t="s">
+        <v>1372</v>
+      </c>
+      <c r="G162">
+        <v>0.38699690402476777</v>
+      </c>
+      <c r="H162">
+        <v>74.029411764705884</v>
+      </c>
+      <c r="I162">
+        <v>0.47368421052631499</v>
+      </c>
+      <c r="J162">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="163" spans="5:10">
+      <c r="F163" t="s">
+        <v>1372</v>
+      </c>
+      <c r="G163">
+        <v>0.38181818181818178</v>
+      </c>
+      <c r="H163">
+        <v>74.890909090909091</v>
+      </c>
+      <c r="I163">
         <v>0.36842105263157898</v>
       </c>
-      <c r="I30">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="33" spans="5:5">
-      <c r="E33" s="13"/>
-    </row>
-    <row r="34" spans="5:5">
-      <c r="E34" s="13"/>
-    </row>
-    <row r="35" spans="5:5">
-      <c r="E35" s="13"/>
-    </row>
-    <row r="36" spans="5:5">
-      <c r="E36" s="13"/>
-    </row>
-    <row r="37" spans="5:5">
-      <c r="E37" s="13"/>
-    </row>
-    <row r="38" spans="5:5">
-      <c r="E38" s="13"/>
-    </row>
-    <row r="39" spans="5:5">
-      <c r="E39" s="13"/>
-    </row>
-    <row r="40" spans="5:5">
-      <c r="E40" s="13"/>
+      <c r="J163">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="164" spans="5:10">
+      <c r="F164" t="s">
+        <v>1372</v>
+      </c>
+      <c r="G164">
+        <v>0.37684210526315792</v>
+      </c>
+      <c r="H164">
+        <v>75.61333333333333</v>
+      </c>
+      <c r="I164">
+        <v>0.42105263157894701</v>
+      </c>
+      <c r="J164">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="165" spans="5:10">
+      <c r="F165" t="s">
+        <v>1372</v>
+      </c>
+      <c r="G165">
+        <v>0.37847427557658198</v>
+      </c>
+      <c r="H165">
+        <v>74.561797752808985</v>
+      </c>
+      <c r="I165">
+        <v>0.36842105263157898</v>
+      </c>
+      <c r="J165">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="166" spans="5:10">
+      <c r="F166" t="s">
+        <v>1372</v>
+      </c>
+      <c r="G166">
+        <v>0.37794486215538842</v>
+      </c>
+      <c r="H166">
+        <v>73.647619047619045</v>
+      </c>
+      <c r="I166">
+        <v>0.31578947368421001</v>
+      </c>
+      <c r="J166">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="167" spans="5:10">
+      <c r="F167" t="s">
+        <v>1372</v>
+      </c>
+      <c r="G167">
+        <v>0.3802631578947368</v>
+      </c>
+      <c r="H167">
+        <v>73.041666666666671</v>
+      </c>
+      <c r="I167">
+        <v>0.42105263157894701</v>
+      </c>
+      <c r="J167">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="168" spans="5:10">
+      <c r="F168" t="s">
+        <v>1372</v>
+      </c>
+      <c r="G168">
+        <v>0.37948131197559121</v>
+      </c>
+      <c r="H168">
+        <v>71.985507246376812</v>
+      </c>
+      <c r="I168">
+        <v>0.36842105263157898</v>
+      </c>
+      <c r="J168">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="169" spans="5:10">
+      <c r="F169" t="s">
+        <v>1372</v>
+      </c>
+      <c r="G169">
+        <v>0.37860780984719872</v>
+      </c>
+      <c r="H169">
+        <v>71.806451612903231</v>
+      </c>
+      <c r="I169">
+        <v>0.36842105263157898</v>
+      </c>
+      <c r="J169">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="170" spans="5:10">
+      <c r="F170" t="s">
+        <v>1372</v>
+      </c>
+      <c r="G170">
+        <v>0.37925696594427238</v>
+      </c>
+      <c r="H170">
+        <v>72.005882352941171</v>
+      </c>
+      <c r="I170">
+        <v>0.31578947368421001</v>
+      </c>
+      <c r="J170">
+        <v>72</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>